<commit_message>
getting a better speed for t49
</commit_message>
<xml_diff>
--- a/track_data/TACK DATA.xlsx
+++ b/track_data/TACK DATA.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Documents\Projects\trains\track_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10200"/>
   </bookViews>
   <sheets>
-    <sheet name="t48s12" sheetId="1" r:id="rId1"/>
+    <sheet name="t49s12" sheetId="1" r:id="rId1"/>
     <sheet name="t50s12" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="90">
   <si>
     <t>C4</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>v_adjusted</t>
+  </si>
+  <si>
+    <t>stop 12</t>
+  </si>
+  <si>
+    <t>stop 8</t>
+  </si>
+  <si>
+    <t>stop 10</t>
   </si>
 </sst>
 </file>
@@ -603,15 +612,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -663,8 +672,11 @@
       <c r="S1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -688,7 +700,7 @@
         <v>712</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:I2" si="1">$C2/F2*10</f>
+        <f t="shared" ref="G2" si="1">$C2/F2*10</f>
         <v>8.7780898876404496</v>
       </c>
       <c r="H2">
@@ -725,8 +737,11 @@
       <c r="S2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>B2</f>
         <v>C8</v>
@@ -763,7 +778,7 @@
         <v>54.75524475524476</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:L31" si="6">AVERAGE(E3,G3,I3)</f>
+        <f t="shared" ref="K3:K31" si="6">AVERAGE(E3,G3,I3)</f>
         <v>47.413759424932607</v>
       </c>
       <c r="L3">
@@ -789,7 +804,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A18" si="8">B3</f>
         <v>A12</v>
@@ -851,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="8"/>
         <v>A16</v>
@@ -914,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="8"/>
         <v>C13</v>
@@ -976,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="8"/>
         <v>E7</v>
@@ -1038,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="8"/>
         <v>D7</v>
@@ -1101,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="8"/>
         <v>D9</v>
@@ -1163,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="8"/>
         <v>E12</v>
@@ -1226,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="8"/>
         <v>D11</v>
@@ -1288,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="8"/>
         <v>C16</v>
@@ -1351,7 +1366,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N13" t="s">
         <v>48</v>
       </c>
@@ -1371,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1390,7 +1405,7 @@
         <v>54.594594594594597</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F42" si="9">SUMIF(P$1:P$80, $B14, Q$1:Q$80)</f>
+        <f t="shared" ref="F14" si="9">SUMIF(P$1:P$80, $B14, Q$1:Q$80)</f>
         <v>74</v>
       </c>
       <c r="G14">
@@ -1398,7 +1413,7 @@
         <v>54.594594594594597</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:H42" si="10">SUMIF(R$1:R$80, $B14, S$1:S$80)</f>
+        <f t="shared" ref="H14" si="10">SUMIF(R$1:R$80, $B14, S$1:S$80)</f>
         <v>74</v>
       </c>
       <c r="I14">
@@ -1432,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N15" t="s">
         <v>50</v>
       </c>
@@ -1452,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1471,7 +1486,7 @@
         <v>57.428571428571431</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F44" si="11">SUMIF(P$1:P$80, $B16, Q$1:Q$80)</f>
+        <f t="shared" ref="F16:F31" si="11">SUMIF(P$1:P$80, $B16, Q$1:Q$80)</f>
         <v>35</v>
       </c>
       <c r="G16">
@@ -1479,7 +1494,7 @@
         <v>57.428571428571431</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H44" si="12">SUMIF(R$1:R$80, $B16, S$1:S$80)</f>
+        <f t="shared" ref="H16:H31" si="12">SUMIF(R$1:R$80, $B16, S$1:S$80)</f>
         <v>35</v>
       </c>
       <c r="I16">
@@ -1702,7 +1717,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f>B19</f>
+        <f t="shared" ref="A20:A31" si="13">B19</f>
         <v>D6</v>
       </c>
       <c r="B20" t="s">
@@ -1765,7 +1780,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f>B20</f>
+        <f t="shared" si="13"/>
         <v>E10</v>
       </c>
       <c r="B21" t="s">
@@ -1827,7 +1842,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f>B21</f>
+        <f t="shared" si="13"/>
         <v>E13</v>
       </c>
       <c r="B22" t="s">
@@ -1890,7 +1905,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f>B22</f>
+        <f t="shared" si="13"/>
         <v>D13</v>
       </c>
       <c r="B23" t="s">
@@ -1952,7 +1967,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
-        <f>B23</f>
+        <f t="shared" si="13"/>
         <v>B2</v>
       </c>
       <c r="B24" t="s">
@@ -2015,7 +2030,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
-        <f>B24</f>
+        <f t="shared" si="13"/>
         <v>C9</v>
       </c>
       <c r="B25" t="s">
@@ -2078,7 +2093,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
-        <f>B25</f>
+        <f t="shared" si="13"/>
         <v>B15</v>
       </c>
       <c r="B26" t="s">
@@ -2140,7 +2155,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
-        <f>B26</f>
+        <f t="shared" si="13"/>
         <v>A3</v>
       </c>
       <c r="B27" t="s">
@@ -2203,7 +2218,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
-        <f>B27</f>
+        <f t="shared" si="13"/>
         <v>C11</v>
       </c>
       <c r="B28" t="s">
@@ -2266,7 +2281,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
-        <f>B28</f>
+        <f t="shared" si="13"/>
         <v>E16</v>
       </c>
       <c r="B29" t="s">
@@ -2328,7 +2343,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
-        <f>B29</f>
+        <f t="shared" si="13"/>
         <v>E1</v>
       </c>
       <c r="B30" t="s">
@@ -2391,7 +2406,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
-        <f>B30</f>
+        <f t="shared" si="13"/>
         <v>C1</v>
       </c>
       <c r="B31" t="s">
@@ -3438,15 +3453,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S80"/>
+  <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3498,8 +3513,17 @@
       <c r="S1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3523,7 +3547,7 @@
         <v>108</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:I2" si="1">$C2/F2*10</f>
+        <f t="shared" ref="G2" si="1">$C2/F2*10</f>
         <v>57.870370370370374</v>
       </c>
       <c r="H2">
@@ -3560,8 +3584,17 @@
       <c r="S2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U2">
+        <v>90</v>
+      </c>
+      <c r="V2">
+        <v>58</v>
+      </c>
+      <c r="W2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>B2</f>
         <v>C8</v>
@@ -3623,8 +3656,17 @@
       <c r="S3">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U3">
+        <v>91</v>
+      </c>
+      <c r="V3">
+        <v>61</v>
+      </c>
+      <c r="W3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A18" si="8">B3</f>
         <v>A12</v>
@@ -3685,8 +3727,17 @@
       <c r="S4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U4">
+        <v>85</v>
+      </c>
+      <c r="V4">
+        <v>60</v>
+      </c>
+      <c r="W4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="8"/>
         <v>A16</v>
@@ -3748,8 +3799,17 @@
       <c r="S5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U5">
+        <v>89</v>
+      </c>
+      <c r="V5">
+        <v>59</v>
+      </c>
+      <c r="W5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="8"/>
         <v>C13</v>
@@ -3810,8 +3870,17 @@
       <c r="S6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <v>90</v>
+      </c>
+      <c r="V6">
+        <v>58</v>
+      </c>
+      <c r="W6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="8"/>
         <v>E7</v>
@@ -3872,8 +3941,11 @@
       <c r="S7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="8"/>
         <v>D7</v>
@@ -3935,8 +4007,11 @@
       <c r="S8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="8"/>
         <v>D9</v>
@@ -3997,8 +4072,11 @@
       <c r="S9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="8"/>
         <v>E12</v>
@@ -4060,8 +4138,11 @@
       <c r="S10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="8"/>
         <v>D11</v>
@@ -4122,8 +4203,11 @@
       <c r="S11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="8"/>
         <v>C16</v>
@@ -4185,8 +4269,11 @@
       <c r="S12">
         <v>143</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U12">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N13" t="s">
         <v>48</v>
       </c>
@@ -4205,8 +4292,11 @@
       <c r="S13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U13">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4225,7 +4315,7 @@
         <v>36.727272727272727</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F42" si="9">SUMIF(P$1:P$80, $B14, Q$1:Q$80)</f>
+        <f t="shared" ref="F14" si="9">SUMIF(P$1:P$80, $B14, Q$1:Q$80)</f>
         <v>74</v>
       </c>
       <c r="G14">
@@ -4233,7 +4323,7 @@
         <v>54.594594594594597</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:H42" si="10">SUMIF(R$1:R$80, $B14, S$1:S$80)</f>
+        <f t="shared" ref="H14" si="10">SUMIF(R$1:R$80, $B14, S$1:S$80)</f>
         <v>110</v>
       </c>
       <c r="I14">
@@ -4266,8 +4356,11 @@
       <c r="S14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U14">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="N15" t="s">
         <v>50</v>
       </c>
@@ -4286,8 +4379,11 @@
       <c r="S15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -4306,7 +4402,7 @@
         <v>59.117647058823536</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16:F44" si="11">SUMIF(P$1:P$80, $B16, Q$1:Q$80)</f>
+        <f t="shared" ref="F16:F31" si="11">SUMIF(P$1:P$80, $B16, Q$1:Q$80)</f>
         <v>70</v>
       </c>
       <c r="G16">
@@ -4314,7 +4410,7 @@
         <v>28.714285714285715</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H44" si="12">SUMIF(R$1:R$80, $B16, S$1:S$80)</f>
+        <f t="shared" ref="H16:H31" si="12">SUMIF(R$1:R$80, $B16, S$1:S$80)</f>
         <v>34</v>
       </c>
       <c r="I16">
@@ -4346,6 +4442,9 @@
       </c>
       <c r="S16">
         <v>180</v>
+      </c>
+      <c r="U16">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -4537,7 +4636,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f>B19</f>
+        <f t="shared" ref="A20:A31" si="14">B19</f>
         <v>D6</v>
       </c>
       <c r="B20" t="s">
@@ -4600,7 +4699,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f>B20</f>
+        <f t="shared" si="14"/>
         <v>E10</v>
       </c>
       <c r="B21" t="s">
@@ -4662,7 +4761,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f>B21</f>
+        <f t="shared" si="14"/>
         <v>E13</v>
       </c>
       <c r="B22" t="s">
@@ -4725,7 +4824,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f>B22</f>
+        <f t="shared" si="14"/>
         <v>D13</v>
       </c>
       <c r="B23" t="s">
@@ -4787,7 +4886,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
-        <f>B23</f>
+        <f t="shared" si="14"/>
         <v>B2</v>
       </c>
       <c r="B24" t="s">
@@ -4850,7 +4949,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
-        <f>B24</f>
+        <f t="shared" si="14"/>
         <v>C9</v>
       </c>
       <c r="B25" t="s">
@@ -4913,7 +5012,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
-        <f>B25</f>
+        <f t="shared" si="14"/>
         <v>B15</v>
       </c>
       <c r="B26" t="s">
@@ -4975,7 +5074,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
-        <f>B26</f>
+        <f t="shared" si="14"/>
         <v>A3</v>
       </c>
       <c r="B27" t="s">
@@ -5038,7 +5137,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
-        <f>B27</f>
+        <f t="shared" si="14"/>
         <v>C11</v>
       </c>
       <c r="B28" t="s">
@@ -5101,7 +5200,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
-        <f>B28</f>
+        <f t="shared" si="14"/>
         <v>E16</v>
       </c>
       <c r="B29" t="s">
@@ -5163,7 +5262,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
-        <f>B29</f>
+        <f t="shared" si="14"/>
         <v>E1</v>
       </c>
       <c r="B30" t="s">
@@ -5226,7 +5325,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
-        <f>B30</f>
+        <f t="shared" si="14"/>
         <v>C1</v>
       </c>
       <c r="B31" t="s">

</xml_diff>